<commit_message>
More analysis tweaks and streamlining
</commit_message>
<xml_diff>
--- a/results/israel/data/loi_israel.xlsx
+++ b/results/israel/data/loi_israel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\israel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B607EAF7-6D67-4B71-BC61-E5E168DCB80E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E63A019-317E-4D8A-9BF2-E6F465ADE14C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10665" yWindow="105" windowWidth="17715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,8 +187,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -405,58 +405,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I903"/>
+  <dimension ref="A1:I486"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="25" width="7.625" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="12.625" style="1"/>
+    <col min="1" max="1" width="7.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="25" width="7.625" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="12.625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
@@ -478,15 +478,15 @@
       <c r="G2" s="3">
         <v>11.4771</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
@@ -508,15 +508,15 @@
       <c r="G3" s="3">
         <v>10.943099999999999</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
@@ -538,15 +538,15 @@
       <c r="G4" s="3">
         <v>10.563000000000001</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
@@ -568,15 +568,15 @@
       <c r="G5" s="3">
         <v>11.602399999999999</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
@@ -598,15 +598,15 @@
       <c r="G6" s="3">
         <v>10.970599999999999</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3">
@@ -628,15 +628,15 @@
       <c r="G7" s="3">
         <v>10.330299999999999</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
@@ -658,15 +658,15 @@
       <c r="G8" s="3">
         <v>11.295500000000001</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
@@ -688,15 +688,15 @@
       <c r="G9" s="3">
         <v>11.349</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3">
@@ -718,15 +718,15 @@
       <c r="G10" s="3">
         <v>9.7728999999999999</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3">
@@ -748,15 +748,15 @@
       <c r="G11" s="3">
         <v>10.1637</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3">
@@ -778,15 +778,15 @@
       <c r="G12" s="3">
         <v>10.0116</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3">
@@ -808,15 +808,15 @@
       <c r="G13" s="3">
         <v>11.1099</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3">
@@ -838,15 +838,15 @@
       <c r="G14" s="3">
         <v>9.8491</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3">
@@ -868,15 +868,15 @@
       <c r="G15" s="3">
         <v>11.143599999999999</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3">
@@ -898,15 +898,15 @@
       <c r="G16" s="3">
         <v>10.421200000000001</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3">
@@ -928,15 +928,15 @@
       <c r="G17" s="3">
         <v>11.165800000000001</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3">
@@ -958,15 +958,15 @@
       <c r="G18" s="3">
         <v>11.5015</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="3">
@@ -988,15 +988,15 @@
       <c r="G19" s="3">
         <v>10.7502</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3">
@@ -1018,10 +1018,10 @@
       <c r="G20" s="3">
         <v>12.3714</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1491,423 +1491,6 @@
     <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>